<commit_message>
Add more Conn College data
</commit_message>
<xml_diff>
--- a/data/college_data.xlsx
+++ b/data/college_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="0" windowWidth="17980" windowHeight="16320" tabRatio="500"/>
+    <workbookView xWindow="620" yWindow="0" windowWidth="18980" windowHeight="16320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2883" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2803" uniqueCount="35">
   <si>
     <t>college</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>https://www.hamilton.edu/oir/common-data-sets</t>
+  </si>
+  <si>
+    <t>very_important</t>
   </si>
 </sst>
 </file>
@@ -579,10 +582,10 @@
   <dimension ref="A1:H1602"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B487" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B490" sqref="B490"/>
+      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8639,16 +8642,16 @@
         <v>2005</v>
       </c>
       <c r="C403" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D403" t="s">
         <v>10</v>
       </c>
-      <c r="E403" t="s">
-        <v>18</v>
-      </c>
-      <c r="F403" t="s">
-        <v>18</v>
+      <c r="E403">
+        <v>0</v>
+      </c>
+      <c r="F403">
+        <v>66</v>
       </c>
     </row>
     <row r="404" spans="1:6">
@@ -8659,16 +8662,16 @@
         <v>2005</v>
       </c>
       <c r="C404" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D404" t="s">
         <v>11</v>
       </c>
-      <c r="E404" t="s">
-        <v>18</v>
-      </c>
-      <c r="F404" t="s">
-        <v>18</v>
+      <c r="E404">
+        <v>14</v>
+      </c>
+      <c r="F404">
+        <v>73</v>
       </c>
     </row>
     <row r="405" spans="1:6">
@@ -8679,16 +8682,16 @@
         <v>2005</v>
       </c>
       <c r="C405" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D405" t="s">
         <v>12</v>
       </c>
-      <c r="E405" t="s">
-        <v>18</v>
-      </c>
-      <c r="F405" t="s">
-        <v>18</v>
+      <c r="E405">
+        <v>0</v>
+      </c>
+      <c r="F405">
+        <v>3</v>
       </c>
     </row>
     <row r="406" spans="1:6">
@@ -8699,16 +8702,16 @@
         <v>2005</v>
       </c>
       <c r="C406" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D406" t="s">
         <v>13</v>
       </c>
-      <c r="E406" t="s">
-        <v>18</v>
-      </c>
-      <c r="F406" t="s">
-        <v>18</v>
+      <c r="E406">
+        <v>28</v>
+      </c>
+      <c r="F406">
+        <v>84</v>
       </c>
     </row>
     <row r="407" spans="1:6">
@@ -8719,16 +8722,16 @@
         <v>2005</v>
       </c>
       <c r="C407" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D407" t="s">
         <v>14</v>
       </c>
-      <c r="E407" t="s">
-        <v>18</v>
-      </c>
-      <c r="F407" t="s">
-        <v>18</v>
+      <c r="E407">
+        <v>26</v>
+      </c>
+      <c r="F407">
+        <v>89</v>
       </c>
     </row>
     <row r="408" spans="1:6">
@@ -8739,16 +8742,16 @@
         <v>2005</v>
       </c>
       <c r="C408" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D408" t="s">
         <v>15</v>
       </c>
-      <c r="E408" t="s">
-        <v>18</v>
-      </c>
-      <c r="F408" t="s">
-        <v>18</v>
+      <c r="E408">
+        <v>376</v>
+      </c>
+      <c r="F408">
+        <v>1304</v>
       </c>
     </row>
     <row r="409" spans="1:6">
@@ -8759,16 +8762,16 @@
         <v>2005</v>
       </c>
       <c r="C409" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D409" t="s">
         <v>16</v>
       </c>
-      <c r="E409" t="s">
-        <v>18</v>
-      </c>
-      <c r="F409" t="s">
-        <v>18</v>
+      <c r="E409">
+        <v>48</v>
+      </c>
+      <c r="F409">
+        <v>159</v>
       </c>
     </row>
     <row r="410" spans="1:6">
@@ -8779,16 +8782,18 @@
         <v>2005</v>
       </c>
       <c r="C410" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D410" t="s">
         <v>17</v>
       </c>
-      <c r="E410" t="s">
-        <v>18</v>
-      </c>
-      <c r="F410" t="s">
-        <v>18</v>
+      <c r="E410">
+        <f>SUM(E403:E409)</f>
+        <v>492</v>
+      </c>
+      <c r="F410">
+        <f>SUM(F403:F409)</f>
+        <v>1778</v>
       </c>
     </row>
     <row r="411" spans="1:6">
@@ -8804,11 +8809,11 @@
       <c r="D411" t="s">
         <v>10</v>
       </c>
-      <c r="E411" t="s">
-        <v>18</v>
-      </c>
-      <c r="F411" t="s">
-        <v>18</v>
+      <c r="E411">
+        <v>22</v>
+      </c>
+      <c r="F411">
+        <v>100</v>
       </c>
     </row>
     <row r="412" spans="1:6">
@@ -8824,11 +8829,11 @@
       <c r="D412" t="s">
         <v>11</v>
       </c>
-      <c r="E412" t="s">
-        <v>18</v>
-      </c>
-      <c r="F412" t="s">
-        <v>18</v>
+      <c r="E412">
+        <v>15</v>
+      </c>
+      <c r="F412">
+        <v>66</v>
       </c>
     </row>
     <row r="413" spans="1:6">
@@ -8844,11 +8849,11 @@
       <c r="D413" t="s">
         <v>12</v>
       </c>
-      <c r="E413" t="s">
-        <v>18</v>
-      </c>
-      <c r="F413" t="s">
-        <v>18</v>
+      <c r="E413">
+        <v>1</v>
+      </c>
+      <c r="F413">
+        <v>2</v>
       </c>
     </row>
     <row r="414" spans="1:6">
@@ -8864,11 +8869,11 @@
       <c r="D414" t="s">
         <v>13</v>
       </c>
-      <c r="E414" t="s">
-        <v>18</v>
-      </c>
-      <c r="F414" t="s">
-        <v>18</v>
+      <c r="E414">
+        <v>15</v>
+      </c>
+      <c r="F414">
+        <v>63</v>
       </c>
     </row>
     <row r="415" spans="1:6">
@@ -8884,11 +8889,11 @@
       <c r="D415" t="s">
         <v>14</v>
       </c>
-      <c r="E415" t="s">
-        <v>18</v>
-      </c>
-      <c r="F415" t="s">
-        <v>18</v>
+      <c r="E415">
+        <v>33</v>
+      </c>
+      <c r="F415">
+        <v>95</v>
       </c>
     </row>
     <row r="416" spans="1:6">
@@ -8904,11 +8909,11 @@
       <c r="D416" t="s">
         <v>15</v>
       </c>
-      <c r="E416" t="s">
-        <v>18</v>
-      </c>
-      <c r="F416" t="s">
-        <v>18</v>
+      <c r="E416">
+        <v>380</v>
+      </c>
+      <c r="F416">
+        <v>1300</v>
       </c>
     </row>
     <row r="417" spans="1:6">
@@ -8924,11 +8929,11 @@
       <c r="D417" t="s">
         <v>16</v>
       </c>
-      <c r="E417" t="s">
-        <v>18</v>
-      </c>
-      <c r="F417" t="s">
-        <v>18</v>
+      <c r="E417">
+        <v>24</v>
+      </c>
+      <c r="F417">
+        <v>134</v>
       </c>
     </row>
     <row r="418" spans="1:6">
@@ -8944,11 +8949,13 @@
       <c r="D418" t="s">
         <v>17</v>
       </c>
-      <c r="E418" t="s">
-        <v>18</v>
-      </c>
-      <c r="F418" t="s">
-        <v>18</v>
+      <c r="E418">
+        <f>SUM(E411:E417)</f>
+        <v>490</v>
+      </c>
+      <c r="F418">
+        <f>SUM(F411:F417)</f>
+        <v>1760</v>
       </c>
     </row>
     <row r="419" spans="1:6">
@@ -8964,11 +8971,11 @@
       <c r="D419" t="s">
         <v>10</v>
       </c>
-      <c r="E419" t="s">
-        <v>18</v>
-      </c>
-      <c r="F419" t="s">
-        <v>18</v>
+      <c r="E419">
+        <v>19</v>
+      </c>
+      <c r="F419">
+        <v>77</v>
       </c>
     </row>
     <row r="420" spans="1:6">
@@ -8984,11 +8991,11 @@
       <c r="D420" t="s">
         <v>11</v>
       </c>
-      <c r="E420" t="s">
-        <v>18</v>
-      </c>
-      <c r="F420" t="s">
-        <v>18</v>
+      <c r="E420">
+        <v>28</v>
+      </c>
+      <c r="F420">
+        <v>71</v>
       </c>
     </row>
     <row r="421" spans="1:6">
@@ -9004,11 +9011,11 @@
       <c r="D421" t="s">
         <v>12</v>
       </c>
-      <c r="E421" t="s">
-        <v>18</v>
-      </c>
-      <c r="F421" t="s">
-        <v>18</v>
+      <c r="E421">
+        <v>0</v>
+      </c>
+      <c r="F421">
+        <v>2</v>
       </c>
     </row>
     <row r="422" spans="1:6">
@@ -9024,11 +9031,11 @@
       <c r="D422" t="s">
         <v>13</v>
       </c>
-      <c r="E422" t="s">
-        <v>18</v>
-      </c>
-      <c r="F422" t="s">
-        <v>18</v>
+      <c r="E422">
+        <v>27</v>
+      </c>
+      <c r="F422">
+        <v>66</v>
       </c>
     </row>
     <row r="423" spans="1:6">
@@ -9044,11 +9051,11 @@
       <c r="D423" t="s">
         <v>14</v>
       </c>
-      <c r="E423" t="s">
-        <v>18</v>
-      </c>
-      <c r="F423" t="s">
-        <v>18</v>
+      <c r="E423">
+        <v>21</v>
+      </c>
+      <c r="F423">
+        <v>92</v>
       </c>
     </row>
     <row r="424" spans="1:6">
@@ -9064,11 +9071,11 @@
       <c r="D424" t="s">
         <v>15</v>
       </c>
-      <c r="E424" t="s">
-        <v>18</v>
-      </c>
-      <c r="F424" t="s">
-        <v>18</v>
+      <c r="E424">
+        <v>370</v>
+      </c>
+      <c r="F424">
+        <v>1308</v>
       </c>
     </row>
     <row r="425" spans="1:6">
@@ -9084,11 +9091,11 @@
       <c r="D425" t="s">
         <v>16</v>
       </c>
-      <c r="E425" t="s">
-        <v>18</v>
-      </c>
-      <c r="F425" t="s">
-        <v>18</v>
+      <c r="E425">
+        <v>27</v>
+      </c>
+      <c r="F425">
+        <v>120</v>
       </c>
     </row>
     <row r="426" spans="1:6">
@@ -9104,11 +9111,13 @@
       <c r="D426" t="s">
         <v>17</v>
       </c>
-      <c r="E426" t="s">
-        <v>18</v>
-      </c>
-      <c r="F426" t="s">
-        <v>18</v>
+      <c r="E426">
+        <f>SUM(E419:E425)</f>
+        <v>492</v>
+      </c>
+      <c r="F426">
+        <f>SUM(F419:F425)</f>
+        <v>1736</v>
       </c>
     </row>
     <row r="427" spans="1:6">
@@ -9119,16 +9128,16 @@
         <v>2008</v>
       </c>
       <c r="C427" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D427" t="s">
         <v>10</v>
       </c>
-      <c r="E427" t="s">
-        <v>18</v>
-      </c>
-      <c r="F427" t="s">
-        <v>18</v>
+      <c r="E427">
+        <v>26</v>
+      </c>
+      <c r="F427">
+        <v>78</v>
       </c>
     </row>
     <row r="428" spans="1:6">
@@ -9139,16 +9148,16 @@
         <v>2008</v>
       </c>
       <c r="C428" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D428" t="s">
         <v>11</v>
       </c>
-      <c r="E428" t="s">
-        <v>18</v>
-      </c>
-      <c r="F428" t="s">
-        <v>18</v>
+      <c r="E428">
+        <v>16</v>
+      </c>
+      <c r="F428">
+        <v>71</v>
       </c>
     </row>
     <row r="429" spans="1:6">
@@ -9159,16 +9168,16 @@
         <v>2008</v>
       </c>
       <c r="C429" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D429" t="s">
         <v>12</v>
       </c>
-      <c r="E429" t="s">
-        <v>18</v>
-      </c>
-      <c r="F429" t="s">
-        <v>18</v>
+      <c r="E429">
+        <v>1</v>
+      </c>
+      <c r="F429">
+        <v>2</v>
       </c>
     </row>
     <row r="430" spans="1:6">
@@ -9179,16 +9188,16 @@
         <v>2008</v>
       </c>
       <c r="C430" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D430" t="s">
         <v>13</v>
       </c>
-      <c r="E430" t="s">
-        <v>18</v>
-      </c>
-      <c r="F430" t="s">
-        <v>18</v>
+      <c r="E430">
+        <v>30</v>
+      </c>
+      <c r="F430">
+        <v>80</v>
       </c>
     </row>
     <row r="431" spans="1:6">
@@ -9199,16 +9208,16 @@
         <v>2008</v>
       </c>
       <c r="C431" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D431" t="s">
         <v>14</v>
       </c>
-      <c r="E431" t="s">
-        <v>18</v>
-      </c>
-      <c r="F431" t="s">
-        <v>18</v>
+      <c r="E431">
+        <v>29</v>
+      </c>
+      <c r="F431">
+        <v>97</v>
       </c>
     </row>
     <row r="432" spans="1:6">
@@ -9219,16 +9228,16 @@
         <v>2008</v>
       </c>
       <c r="C432" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D432" t="s">
         <v>15</v>
       </c>
-      <c r="E432" t="s">
-        <v>18</v>
-      </c>
-      <c r="F432" t="s">
-        <v>18</v>
+      <c r="E432">
+        <v>366</v>
+      </c>
+      <c r="F432">
+        <v>1295</v>
       </c>
     </row>
     <row r="433" spans="1:6">
@@ -9239,16 +9248,16 @@
         <v>2008</v>
       </c>
       <c r="C433" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D433" t="s">
         <v>16</v>
       </c>
-      <c r="E433" t="s">
-        <v>18</v>
-      </c>
-      <c r="F433" t="s">
-        <v>18</v>
+      <c r="E433">
+        <v>25</v>
+      </c>
+      <c r="F433">
+        <v>112</v>
       </c>
     </row>
     <row r="434" spans="1:6">
@@ -9259,16 +9268,16 @@
         <v>2008</v>
       </c>
       <c r="C434" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D434" t="s">
         <v>17</v>
       </c>
-      <c r="E434" t="s">
-        <v>18</v>
-      </c>
-      <c r="F434" t="s">
-        <v>18</v>
+      <c r="E434">
+        <v>493</v>
+      </c>
+      <c r="F434">
+        <v>1735</v>
       </c>
     </row>
     <row r="435" spans="1:6">
@@ -9279,16 +9288,16 @@
         <v>2009</v>
       </c>
       <c r="C435" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D435" t="s">
         <v>10</v>
       </c>
-      <c r="E435" t="s">
-        <v>18</v>
-      </c>
-      <c r="F435" t="s">
-        <v>18</v>
+      <c r="E435">
+        <v>23</v>
+      </c>
+      <c r="F435">
+        <v>69</v>
       </c>
     </row>
     <row r="436" spans="1:6">
@@ -9299,16 +9308,16 @@
         <v>2009</v>
       </c>
       <c r="C436" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D436" t="s">
         <v>11</v>
       </c>
-      <c r="E436" t="s">
-        <v>18</v>
-      </c>
-      <c r="F436" t="s">
-        <v>18</v>
+      <c r="E436">
+        <v>19</v>
+      </c>
+      <c r="F436">
+        <v>73</v>
       </c>
     </row>
     <row r="437" spans="1:6">
@@ -9319,16 +9328,16 @@
         <v>2009</v>
       </c>
       <c r="C437" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D437" t="s">
         <v>12</v>
       </c>
-      <c r="E437" t="s">
-        <v>18</v>
-      </c>
-      <c r="F437" t="s">
-        <v>18</v>
+      <c r="E437">
+        <v>1</v>
+      </c>
+      <c r="F437">
+        <v>4</v>
       </c>
     </row>
     <row r="438" spans="1:6">
@@ -9339,16 +9348,16 @@
         <v>2009</v>
       </c>
       <c r="C438" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D438" t="s">
         <v>13</v>
       </c>
-      <c r="E438" t="s">
-        <v>18</v>
-      </c>
-      <c r="F438" t="s">
-        <v>18</v>
+      <c r="E438">
+        <v>21</v>
+      </c>
+      <c r="F438">
+        <v>84</v>
       </c>
     </row>
     <row r="439" spans="1:6">
@@ -9359,16 +9368,16 @@
         <v>2009</v>
       </c>
       <c r="C439" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D439" t="s">
         <v>14</v>
       </c>
-      <c r="E439" t="s">
-        <v>18</v>
-      </c>
-      <c r="F439" t="s">
-        <v>18</v>
+      <c r="E439">
+        <v>31</v>
+      </c>
+      <c r="F439">
+        <v>101</v>
       </c>
     </row>
     <row r="440" spans="1:6">
@@ -9379,16 +9388,16 @@
         <v>2009</v>
       </c>
       <c r="C440" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D440" t="s">
         <v>15</v>
       </c>
-      <c r="E440" t="s">
-        <v>18</v>
-      </c>
-      <c r="F440" t="s">
-        <v>18</v>
+      <c r="E440">
+        <v>376</v>
+      </c>
+      <c r="F440">
+        <v>1331</v>
       </c>
     </row>
     <row r="441" spans="1:6">
@@ -9399,16 +9408,16 @@
         <v>2009</v>
       </c>
       <c r="C441" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D441" t="s">
         <v>16</v>
       </c>
-      <c r="E441" t="s">
-        <v>18</v>
-      </c>
-      <c r="F441" t="s">
-        <v>18</v>
+      <c r="E441">
+        <v>31</v>
+      </c>
+      <c r="F441">
+        <v>115</v>
       </c>
     </row>
     <row r="442" spans="1:6">
@@ -9419,16 +9428,16 @@
         <v>2009</v>
       </c>
       <c r="C442" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D442" t="s">
         <v>17</v>
       </c>
-      <c r="E442" t="s">
-        <v>18</v>
-      </c>
-      <c r="F442" t="s">
-        <v>18</v>
+      <c r="E442">
+        <v>502</v>
+      </c>
+      <c r="F442">
+        <v>1777</v>
       </c>
     </row>
     <row r="443" spans="1:6">

</xml_diff>